<commit_message>
Add more items to supply list
</commit_message>
<xml_diff>
--- a/Supplies.xlsx
+++ b/Supplies.xlsx
@@ -19,7 +19,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
+  <si>
+    <t>Variable voltage power supply</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Variable voltage power brick</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>12V-24V up to 5A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>power small external components</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>chipKIT Pi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PIC32 microcontroller</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
   <si>
     <t>Distance sensor</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -125,14 +149,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>RaspiRobot</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Robot controller board for Pi</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>IR Proximity Seonsor (long range)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -154,6 +170,70 @@
   </si>
   <si>
     <t>Connect things to the raspberry pi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DC Motors</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Various motors</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">LEDs </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Blue, Yellow, Green and Red</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Various battery connectors</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>9V, 2 AA, 4 AA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Arduino Mega 2560</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Arduino</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Game controllers</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plus 2 that don't work well</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wireless Keyboard/Air mouse</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Keyboard and mouse in the form factor of a remote control</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resistors</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varried resistors</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -533,10 +613,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -548,145 +628,142 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="26">
       <c r="A7" s="2" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B9" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="1">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="13" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="B13" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -700,50 +777,150 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="26">
+    <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="1">
+        <v>4</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="26">
+      <c r="A18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="1">
+        <v>4</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="1">
+        <v>4</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="26">
+      <c r="A24" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="1">
         <v>3</v>
       </c>
-      <c r="B16" s="1">
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="1">
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.59722222222222221" right="0.5" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>